<commit_message>
Added send AT command to WiFi module via JMRI
</commit_message>
<xml_diff>
--- a/src/CommInterface/DCCEX-commands.xlsx
+++ b/src/CommInterface/DCCEX-commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidcutting42\src\CommandStation-DCC\.pio\libdeps\samd21\CommandStation\src\CommInterface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidcutting42\src\dcc-ex\CommandStation-EX\src\CommInterface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128305C1-9278-467E-BF20-D32E87FC58FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA376B75-2878-4F21-988F-D62061E88DEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{03B09B78-E6DF-4BC3-A68B-D67D20DF6376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03B09B78-E6DF-4BC3-A68B-D67D20DF6376}"/>
   </bookViews>
   <sheets>
     <sheet name="DCC++ EX" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="133">
   <si>
     <t>Param 1</t>
   </si>
@@ -419,6 +419,18 @@
   </si>
   <si>
     <t>Read four CVs on main (railcom). Reads cv, cv+1, cv+2, cv+3</t>
+  </si>
+  <si>
+    <t>MAIN/PROG/JOIN</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Send AT Command to WiFi Module</t>
+  </si>
+  <si>
+    <t>string, do not include + or 'AT'</t>
   </si>
 </sst>
 </file>
@@ -792,11 +804,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C789B9-828D-42BA-9B4D-23D02CCD2FAC}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,6 +857,9 @@
       <c r="C2" t="s">
         <v>63</v>
       </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -856,6 +871,9 @@
       <c r="C3" t="s">
         <v>64</v>
       </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1593,6 +1611,20 @@
       </c>
       <c r="C75" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" t="s">
+        <v>131</v>
+      </c>
+      <c r="D76" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>